<commit_message>
added the Philips Irrigation data in the main_irrigation xsls file
</commit_message>
<xml_diff>
--- a/data/irrigation/irrigation_main.xlsx
+++ b/data/irrigation/irrigation_main.xlsx
@@ -1,40 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/ETH/code/cciwr/data/irrigation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jss/cciwr-1/data/irrigation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697773CD-398D-034B-9841-F50C90C696FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41473C6E-21C5-1E4E-BC61-D6939CAFB373}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3660" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{F5263EFD-E13A-114A-926B-CA9CAC78BE47}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="4" xr2:uid="{F5263EFD-E13A-114A-926B-CA9CAC78BE47}"/>
   </bookViews>
   <sheets>
     <sheet name="AEI national" sheetId="4" r:id="rId1"/>
     <sheet name="IWU national" sheetId="3" r:id="rId2"/>
     <sheet name="AEI regional" sheetId="2" r:id="rId3"/>
     <sheet name="Crop Calendars" sheetId="5" r:id="rId4"/>
+    <sheet name="Irrigation demand Philips" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.10" hidden="1">'AEI national'!$C$5</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'AEI national'!$C$6:$C$19</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'AEI national'!$D$5</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'AEI national'!$D$6:$D$19</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'AEI national'!$E$5</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'AEI national'!$E$6:$E$19</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'AEI national'!$B$5</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'AEI national'!$B$6:$B$19</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">'AEI national'!$B$5</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">'AEI national'!$B$6:$B$19</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">'AEI national'!$C$5</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">'AEI national'!$C$6:$C$19</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">'AEI national'!$D$5</definedName>
-    <definedName name="_xlchart.v2.5" hidden="1">'AEI national'!$D$6:$D$19</definedName>
-    <definedName name="_xlchart.v2.6" hidden="1">'AEI national'!$E$5</definedName>
-    <definedName name="_xlchart.v2.7" hidden="1">'AEI national'!$E$6:$E$19</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'AEI regional'!$1:$2</definedName>
     <definedName name="test">#REF!</definedName>
   </definedNames>
@@ -56,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t>index</t>
   </si>
@@ -413,6 +398,81 @@
   </si>
   <si>
     <t>http://www.fao.org/nr/water/aquastat/water_use_agr/IrrigationWaterUse.pdf</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1XoxDHWwr7wy2YkkLW0hgJynG-NyjEeHn</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ilisu irrigation demand  </t>
+  </si>
+  <si>
+    <t>513000 [ha]</t>
+  </si>
+  <si>
+    <t>121000 [ha]</t>
+  </si>
+  <si>
+    <t>138287 [ha]</t>
+  </si>
+  <si>
+    <t>Upstream use (existing) [m3/s]</t>
+  </si>
+  <si>
+    <t>Upstream use (planned) [m3/s]</t>
+  </si>
+  <si>
+    <t>Downstream use (existing) [m3/s]</t>
+  </si>
+  <si>
+    <t>Mean flow [m3/s]</t>
+  </si>
+  <si>
+    <t>Inflow Ilisu (existing) [m3/s]</t>
+  </si>
+  <si>
+    <t>Inflow Ilisu (planned) [m3/s]</t>
+  </si>
+  <si>
+    <t>Outflow Ilisu [m3/s]</t>
   </si>
 </sst>
 </file>
@@ -422,7 +482,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###\ ###\ ###\ ##0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -433,10 +493,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8.5"/>
@@ -467,6 +529,20 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -531,7 +607,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -553,6 +629,18 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -574,18 +662,10 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -670,7 +750,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-AT"/>
+          <a:endParaRPr lang="en-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1187,7 +1267,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-AT"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1038218912"/>
@@ -1249,7 +1329,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-AT"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1038217280"/>
@@ -1291,7 +1371,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-AT"/>
+          <a:endParaRPr lang="en-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1321,7 +1401,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-AT"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2232,28 +2312,28 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C5" t="s">
@@ -2265,33 +2345,33 @@
       <c r="E5" t="s">
         <v>109</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="17">
         <v>1900</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="15">
         <v>603174</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="15">
         <v>65000</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="15">
         <v>403230</v>
       </c>
       <c r="F6" s="1"/>
@@ -2307,11 +2387,11 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>11</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="17">
         <v>1910</v>
       </c>
       <c r="C7" s="1">
@@ -2323,24 +2403,24 @@
       <c r="E7" s="1">
         <v>452510</v>
       </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>21</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="17">
         <v>1920</v>
       </c>
       <c r="C8" s="1">
@@ -2352,24 +2432,24 @@
       <c r="E8" s="1">
         <v>501790</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>31</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="17">
         <v>1930</v>
       </c>
       <c r="C9" s="1">
@@ -2382,11 +2462,11 @@
         <v>551080</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>41</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="17">
         <v>1940</v>
       </c>
       <c r="C10" s="1">
@@ -2399,11 +2479,11 @@
         <v>600360</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>51</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="17">
         <v>1950</v>
       </c>
       <c r="C11" s="1">
@@ -2416,11 +2496,11 @@
         <v>820310</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>61</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="17">
         <v>1960</v>
       </c>
       <c r="C12" s="1">
@@ -2433,11 +2513,11 @@
         <v>1224444.44</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>71</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="17">
         <v>1970</v>
       </c>
       <c r="C13" s="1">
@@ -2450,11 +2530,11 @@
         <v>1480000</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>81</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="17">
         <v>1980</v>
       </c>
       <c r="C14" s="1">
@@ -2467,11 +2547,11 @@
         <v>1750000</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>86</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="17">
         <v>1985</v>
       </c>
       <c r="C15" s="1">
@@ -2484,11 +2564,11 @@
         <v>1750000</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>91</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="17">
         <v>1990</v>
       </c>
       <c r="C16" s="1">
@@ -2501,11 +2581,11 @@
         <v>3525000</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>96</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="17">
         <v>1995</v>
       </c>
       <c r="C17" s="1">
@@ -2518,11 +2598,11 @@
         <v>3525000</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>101</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="17">
         <v>2000</v>
       </c>
       <c r="C18" s="1">
@@ -2535,11 +2615,11 @@
         <v>3525000</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>106</v>
       </c>
-      <c r="B19" s="24">
+      <c r="B19" s="17">
         <v>2005</v>
       </c>
       <c r="C19" s="1">
@@ -2569,24 +2649,24 @@
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -2609,14 +2689,14 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>99</v>
       </c>
       <c r="B6" s="1">
         <v>213600</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="18">
         <v>2006</v>
       </c>
       <c r="D6" s="1">
@@ -2632,14 +2712,14 @@
         <v>13.86</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>100</v>
       </c>
       <c r="B7" s="1">
         <v>75610</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="18">
         <v>1990</v>
       </c>
       <c r="D7" s="1">
@@ -2655,14 +2735,14 @@
         <v>68.77</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>101</v>
       </c>
       <c r="B8" s="1">
         <v>16800</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="18">
         <v>2004</v>
       </c>
       <c r="D8" s="1">
@@ -2695,7 +2775,7 @@
       <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" style="5" bestFit="1" customWidth="1"/>
@@ -2706,25 +2786,25 @@
     <col min="7" max="16384" width="11.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="14" t="s">
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="20" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A2" s="19"/>
-      <c r="B2" s="17"/>
+    <row r="2" spans="1:6" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="25"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="11" t="s">
         <v>86</v>
       </c>
@@ -2734,9 +2814,9 @@
       <c r="E2" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="15"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2" s="21"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>83</v>
       </c>
@@ -2756,7 +2836,7 @@
         <v>172209.1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>82</v>
       </c>
@@ -2776,7 +2856,7 @@
         <v>35863</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>81</v>
       </c>
@@ -2796,7 +2876,7 @@
         <v>42625.2</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>80</v>
       </c>
@@ -2816,7 +2896,7 @@
         <v>54879</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
         <v>79</v>
       </c>
@@ -2836,7 +2916,7 @@
         <v>30008</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>78</v>
       </c>
@@ -2856,7 +2936,7 @@
         <v>41441.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
         <v>77</v>
       </c>
@@ -2876,7 +2956,7 @@
         <v>34838.5</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
         <v>76</v>
       </c>
@@ -2896,7 +2976,7 @@
         <v>75528.600000000006</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
         <v>75</v>
       </c>
@@ -2916,7 +2996,7 @@
         <v>2070.1999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
         <v>74</v>
       </c>
@@ -2936,7 +3016,7 @@
         <v>15724</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
         <v>73</v>
       </c>
@@ -2956,7 +3036,7 @@
         <v>114864.4</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
         <v>72</v>
       </c>
@@ -2976,7 +3056,7 @@
         <v>55543.3</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
         <v>71</v>
       </c>
@@ -2996,7 +3076,7 @@
         <v>1661.1</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
         <v>70</v>
       </c>
@@ -3016,7 +3096,7 @@
         <v>9056.9</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
         <v>69</v>
       </c>
@@ -3036,7 +3116,7 @@
         <v>15170.9</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
         <v>68</v>
       </c>
@@ -3056,7 +3136,7 @@
         <v>5933.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
         <v>67</v>
       </c>
@@ -3076,7 +3156,7 @@
         <v>22873</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
         <v>66</v>
       </c>
@@ -3096,7 +3176,7 @@
         <v>18828.900000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
         <v>65</v>
       </c>
@@ -3116,7 +3196,7 @@
         <v>6633.2</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
         <v>64</v>
       </c>
@@ -3136,7 +3216,7 @@
         <v>31946.400000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
         <v>63</v>
       </c>
@@ -3156,7 +3236,7 @@
         <v>71149.3</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
         <v>62</v>
       </c>
@@ -3176,7 +3256,7 @@
         <v>52381.5</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
         <v>61</v>
       </c>
@@ -3196,7 +3276,7 @@
         <v>14254.1</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
         <v>60</v>
       </c>
@@ -3216,7 +3296,7 @@
         <v>28808.799999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
         <v>59</v>
       </c>
@@ -3236,7 +3316,7 @@
         <v>102115</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" s="5" t="s">
         <v>58</v>
       </c>
@@ -3256,7 +3336,7 @@
         <v>42597.1</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
         <v>57</v>
       </c>
@@ -3276,7 +3356,7 @@
         <v>7695.4</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" s="6" t="s">
         <v>56</v>
       </c>
@@ -3296,7 +3376,7 @@
         <v>32298.6</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" s="5" t="s">
         <v>55</v>
       </c>
@@ -3316,7 +3396,7 @@
         <v>48301.599999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" s="6" t="s">
         <v>54</v>
       </c>
@@ -3336,7 +3416,7 @@
         <v>38637.4</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
         <v>53</v>
       </c>
@@ -3356,7 +3436,7 @@
         <v>116251.3</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
         <v>52</v>
       </c>
@@ -3376,7 +3456,7 @@
         <v>66633.399999999994</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" s="6" t="s">
         <v>51</v>
       </c>
@@ -3396,7 +3476,7 @@
         <v>50066</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" s="6" t="s">
         <v>50</v>
       </c>
@@ -3416,7 +3496,7 @@
         <v>3616</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" s="5" t="s">
         <v>49</v>
       </c>
@@ -3436,7 +3516,7 @@
         <v>8030.7</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="s">
         <v>48</v>
       </c>
@@ -3456,7 +3536,7 @@
         <v>22965.599999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39" s="6" t="s">
         <v>47</v>
       </c>
@@ -3476,7 +3556,7 @@
         <v>91256.5</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40" s="5" t="s">
         <v>46</v>
       </c>
@@ -3496,7 +3576,7 @@
         <v>35822.1</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41" s="6" t="s">
         <v>45</v>
       </c>
@@ -3516,7 +3596,7 @@
         <v>31727.7</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42" s="5" t="s">
         <v>44</v>
       </c>
@@ -3536,7 +3616,7 @@
         <v>4059.8</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" s="5" t="s">
         <v>43</v>
       </c>
@@ -3556,7 +3636,7 @@
         <v>132774.79999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" s="5" t="s">
         <v>42</v>
       </c>
@@ -3576,7 +3656,7 @@
         <v>122866.7</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" s="5" t="s">
         <v>41</v>
       </c>
@@ -3596,7 +3676,7 @@
         <v>2346.8000000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" s="6" t="s">
         <v>40</v>
       </c>
@@ -3616,7 +3696,7 @@
         <v>35136</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" s="6" t="s">
         <v>39</v>
       </c>
@@ -3636,7 +3716,7 @@
         <v>5028.1000000000004</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" s="6" t="s">
         <v>38</v>
       </c>
@@ -3656,7 +3736,7 @@
         <v>19000.7</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" s="6" t="s">
         <v>37</v>
       </c>
@@ -3676,7 +3756,7 @@
         <v>35157</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A50" s="6" t="s">
         <v>36</v>
       </c>
@@ -3696,7 +3776,7 @@
         <v>3796.3</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A51" s="5" t="s">
         <v>35</v>
       </c>
@@ -3716,7 +3796,7 @@
         <v>5638.7</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" s="5" t="s">
         <v>34</v>
       </c>
@@ -3736,7 +3816,7 @@
         <v>11453.4</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A53" s="5" t="s">
         <v>33</v>
       </c>
@@ -3756,7 +3836,7 @@
         <v>15145.3</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54" s="6" t="s">
         <v>32</v>
       </c>
@@ -3776,7 +3856,7 @@
         <v>4098.5</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A55" s="6" t="s">
         <v>31</v>
       </c>
@@ -3796,7 +3876,7 @@
         <v>292413.8</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A56" s="5" t="s">
         <v>30</v>
       </c>
@@ -3816,7 +3896,7 @@
         <v>11651.7</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A57" s="6" t="s">
         <v>29</v>
       </c>
@@ -3836,7 +3916,7 @@
         <v>78753.899999999994</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A58" s="6" t="s">
         <v>28</v>
       </c>
@@ -3856,7 +3936,7 @@
         <v>113761.2</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59" s="6" t="s">
         <v>27</v>
       </c>
@@ -3876,7 +3956,7 @@
         <v>50143.3</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A60" s="6" t="s">
         <v>26</v>
       </c>
@@ -3896,7 +3976,7 @@
         <v>99291.8</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A61" s="5" t="s">
         <v>25</v>
       </c>
@@ -3916,7 +3996,7 @@
         <v>39595.4</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A62" s="5" t="s">
         <v>24</v>
       </c>
@@ -3936,7 +4016,7 @@
         <v>27078.6</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A63" s="5" t="s">
         <v>23</v>
       </c>
@@ -3956,7 +4036,7 @@
         <v>28056.1</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A64" s="5" t="s">
         <v>22</v>
       </c>
@@ -3976,7 +4056,7 @@
         <v>48464.800000000003</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A65" s="6" t="s">
         <v>21</v>
       </c>
@@ -3996,7 +4076,7 @@
         <v>373.4</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66" s="6" t="s">
         <v>20</v>
       </c>
@@ -4016,7 +4096,7 @@
         <v>35394.5</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A67" s="6" t="s">
         <v>19</v>
       </c>
@@ -4036,7 +4116,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A68" s="6" t="s">
         <v>18</v>
       </c>
@@ -4056,7 +4136,7 @@
         <v>20139.900000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A69" s="6" t="s">
         <v>17</v>
       </c>
@@ -4076,7 +4156,7 @@
         <v>51872.5</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A70" s="5" t="s">
         <v>16</v>
       </c>
@@ -4096,7 +4176,7 @@
         <v>247750.5</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71" s="6" t="s">
         <v>15</v>
       </c>
@@ -4116,7 +4196,7 @@
         <v>15788.1</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A72" s="6" t="s">
         <v>14</v>
       </c>
@@ -4136,7 +4216,7 @@
         <v>11847.9</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A73" s="5" t="s">
         <v>13</v>
       </c>
@@ -4156,7 +4236,7 @@
         <v>14427</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A74" s="6" t="s">
         <v>12</v>
       </c>
@@ -4176,7 +4256,7 @@
         <v>25256.400000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75" s="5" t="s">
         <v>11</v>
       </c>
@@ -4196,7 +4276,7 @@
         <v>3059.9</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A76" s="6" t="s">
         <v>10</v>
       </c>
@@ -4216,7 +4296,7 @@
         <v>35734.1</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A77" s="6" t="s">
         <v>9</v>
       </c>
@@ -4236,7 +4316,7 @@
         <v>976.1</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A78" s="6" t="s">
         <v>8</v>
       </c>
@@ -4256,7 +4336,7 @@
         <v>10799.7</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A79" s="5" t="s">
         <v>7</v>
       </c>
@@ -4276,7 +4356,7 @@
         <v>3136.5</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A80" s="6" t="s">
         <v>6</v>
       </c>
@@ -4296,7 +4376,7 @@
         <v>73154.3</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A81" s="6" t="s">
         <v>5</v>
       </c>
@@ -4316,7 +4396,7 @@
         <v>2525.5</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A82" s="6" t="s">
         <v>4</v>
       </c>
@@ -4336,7 +4416,7 @@
         <v>22583.5</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="13" thickBot="1">
+    <row r="83" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>3</v>
       </c>
@@ -4356,7 +4436,7 @@
         <v>2299.5</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="14" thickTop="1" thickBot="1">
+    <row r="84" spans="1:6" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A84" s="8" t="s">
         <v>2</v>
       </c>
@@ -4381,127 +4461,127 @@
         <v>3415143.8</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="13" thickTop="1">
+    <row r="85" spans="1:6" ht="13" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A85" s="6"/>
       <c r="B85" s="4"/>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A86" s="6"/>
       <c r="B86" s="4"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A87" s="6"/>
       <c r="B87" s="4"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A88" s="6"/>
       <c r="B88" s="4"/>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A89" s="6"/>
       <c r="B89" s="4"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A90" s="6"/>
       <c r="B90" s="4"/>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A91" s="6"/>
       <c r="B91" s="4"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A92" s="6"/>
       <c r="B92" s="4"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A93" s="6"/>
       <c r="B93" s="4"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A94" s="6"/>
       <c r="B94" s="4"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A95" s="6"/>
       <c r="B95" s="4"/>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A96" s="6"/>
       <c r="B96" s="4"/>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A97" s="6"/>
       <c r="B97" s="4"/>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A98" s="6"/>
       <c r="B98" s="4"/>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A99" s="6"/>
       <c r="B99" s="4"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A100" s="6"/>
       <c r="B100" s="4"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A101" s="6"/>
       <c r="B101" s="4"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A102" s="6"/>
       <c r="B102" s="4"/>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A103" s="6"/>
       <c r="B103" s="4"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A104" s="6"/>
       <c r="B104" s="4"/>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A105" s="6"/>
       <c r="B105" s="4"/>
       <c r="C105" s="3"/>
@@ -4531,209 +4611,209 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A78E96B0-42F0-1543-ABF1-5763666B8AE4}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.83203125" customWidth="1"/>
     <col min="2" max="2" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>117</v>
       </c>
       <c r="B5" t="s">
         <v>115</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="18">
         <v>1</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="18">
         <v>2</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="18">
         <v>3</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="18">
         <v>4</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="18">
         <v>5</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="18">
         <v>6</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="18">
         <v>7</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="18">
         <v>8</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="18">
         <v>9</v>
       </c>
-      <c r="L5" s="25">
+      <c r="L5" s="18">
         <v>10</v>
       </c>
-      <c r="M5" s="25">
+      <c r="M5" s="18">
         <v>11</v>
       </c>
-      <c r="N5" s="25">
+      <c r="N5" s="18">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="18">
         <v>4206000</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="18">
         <v>25</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="18">
         <v>25</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="18">
         <v>25</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="18">
         <v>48</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="18">
         <v>100</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="18">
         <v>94</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="18">
         <v>94</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6" s="18">
         <v>94</v>
       </c>
-      <c r="K6" s="25">
+      <c r="K6" s="18">
         <v>94</v>
       </c>
-      <c r="L6" s="25">
+      <c r="L6" s="18">
         <v>35</v>
       </c>
-      <c r="M6" s="25">
+      <c r="M6" s="18">
         <v>25</v>
       </c>
-      <c r="N6" s="25">
+      <c r="N6" s="18">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>112</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="18">
         <v>2050000</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="18">
         <v>99</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="18">
         <v>99</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="18">
         <v>99</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="18">
         <v>100</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="18">
         <v>47</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="18">
         <v>47</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="18">
         <v>47</v>
       </c>
-      <c r="J7" s="25">
+      <c r="J7" s="18">
         <v>47</v>
       </c>
-      <c r="K7" s="25">
+      <c r="K7" s="18">
         <v>47</v>
       </c>
-      <c r="L7" s="25">
+      <c r="L7" s="18">
         <v>77</v>
       </c>
-      <c r="M7" s="25">
+      <c r="M7" s="18">
         <v>99</v>
       </c>
-      <c r="N7" s="25">
+      <c r="N7" s="18">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>114</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="18">
         <v>1334000</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="18">
         <v>76</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="18">
         <v>76</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="18">
         <v>76</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="18">
         <v>76</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="18">
         <v>92</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="18">
         <v>45</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="18">
         <v>45</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J8" s="18">
         <v>45</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K8" s="18">
         <v>45</v>
       </c>
-      <c r="L8" s="25">
+      <c r="L8" s="18">
         <v>45</v>
       </c>
-      <c r="M8" s="25">
+      <c r="M8" s="18">
         <v>98</v>
       </c>
-      <c r="N8" s="25">
+      <c r="N8" s="18">
         <v>76</v>
       </c>
     </row>
@@ -4743,4 +4823,402 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87D1705-F5B2-D54D-9AA4-BAACB3065371}">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" customWidth="1"/>
+    <col min="7" max="7" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="12"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C4" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="H4" s="27"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6">
+        <v>138.49</v>
+      </c>
+      <c r="C6">
+        <v>14.51</v>
+      </c>
+      <c r="D6">
+        <v>123.98</v>
+      </c>
+      <c r="E6">
+        <v>53.83</v>
+      </c>
+      <c r="F6">
+        <v>84.66</v>
+      </c>
+      <c r="G6">
+        <v>12.7</v>
+      </c>
+      <c r="H6">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7">
+        <v>229.27</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>229.27</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>229.27</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8">
+        <v>362.87</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>362.87</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>362.87</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9">
+        <v>346.68</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>346.68</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>346.68</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10">
+        <v>529.48</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>529.48</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>529.48</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11">
+        <v>903</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>903</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>903</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12">
+        <v>1337.17</v>
+      </c>
+      <c r="C12">
+        <v>35</v>
+      </c>
+      <c r="D12">
+        <v>1302.17</v>
+      </c>
+      <c r="E12">
+        <v>129.83000000000001</v>
+      </c>
+      <c r="F12">
+        <v>1207.3399999999999</v>
+      </c>
+      <c r="G12">
+        <v>30.62</v>
+      </c>
+      <c r="H12">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13">
+        <v>1063.58</v>
+      </c>
+      <c r="C13">
+        <v>70.86</v>
+      </c>
+      <c r="D13">
+        <v>992.72</v>
+      </c>
+      <c r="E13">
+        <v>262.83</v>
+      </c>
+      <c r="F13">
+        <v>800.75</v>
+      </c>
+      <c r="G13">
+        <v>61.99</v>
+      </c>
+      <c r="H13">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14">
+        <v>455.91</v>
+      </c>
+      <c r="C14">
+        <v>178.42</v>
+      </c>
+      <c r="D14">
+        <v>277.49</v>
+      </c>
+      <c r="E14">
+        <v>661.83</v>
+      </c>
+      <c r="F14">
+        <v>-205.92</v>
+      </c>
+      <c r="G14">
+        <v>156.1</v>
+      </c>
+      <c r="H14">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15">
+        <v>189.26</v>
+      </c>
+      <c r="C15">
+        <v>246.72</v>
+      </c>
+      <c r="D15">
+        <v>-57.46</v>
+      </c>
+      <c r="E15">
+        <v>915.17</v>
+      </c>
+      <c r="F15">
+        <v>-725.91</v>
+      </c>
+      <c r="G15">
+        <v>215.86</v>
+      </c>
+      <c r="H15">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16">
+        <v>113.7</v>
+      </c>
+      <c r="C16">
+        <v>208.3</v>
+      </c>
+      <c r="D16">
+        <v>-94.6</v>
+      </c>
+      <c r="E16">
+        <v>772.67</v>
+      </c>
+      <c r="F16">
+        <v>-658.97</v>
+      </c>
+      <c r="G16">
+        <v>182.25</v>
+      </c>
+      <c r="H16">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17">
+        <v>101.17</v>
+      </c>
+      <c r="C17">
+        <v>99.88</v>
+      </c>
+      <c r="D17">
+        <v>1.29</v>
+      </c>
+      <c r="E17">
+        <v>370.5</v>
+      </c>
+      <c r="F17">
+        <v>-269.33</v>
+      </c>
+      <c r="G17">
+        <v>87.39</v>
+      </c>
+      <c r="H17">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="G4:H4"/>
+  </mergeCells>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{E8E39936-6B26-AB40-9692-EE67A30A2753}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>